<commit_message>
update all project files
</commit_message>
<xml_diff>
--- a/alephnum2rlid_trent_hom_dataset.xlsx
+++ b/alephnum2rlid_trent_hom_dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nh48\Desktop\trenthom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nh48\Documents\GitHub\trenthom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3884" uniqueCount="3863">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3888" uniqueCount="3867">
   <si>
     <t>alephnum</t>
   </si>
@@ -9286,66 +9286,6 @@
     <t>trent-zimmermanjohanngeorg</t>
   </si>
   <si>
-    <t>RL.10180</t>
-  </si>
-  <si>
-    <t>RL.10181</t>
-  </si>
-  <si>
-    <t>RL.10182</t>
-  </si>
-  <si>
-    <t>RL.10183</t>
-  </si>
-  <si>
-    <t>RL.10184</t>
-  </si>
-  <si>
-    <t>RL.10185</t>
-  </si>
-  <si>
-    <t>RL.10186</t>
-  </si>
-  <si>
-    <t>RL.10187</t>
-  </si>
-  <si>
-    <t>RL.10188</t>
-  </si>
-  <si>
-    <t>RL.10189</t>
-  </si>
-  <si>
-    <t>RL.10190</t>
-  </si>
-  <si>
-    <t>RL.10191</t>
-  </si>
-  <si>
-    <t>RL.10192</t>
-  </si>
-  <si>
-    <t>RL.10193</t>
-  </si>
-  <si>
-    <t>RL.10194</t>
-  </si>
-  <si>
-    <t>RL.10195</t>
-  </si>
-  <si>
-    <t>RL.10196</t>
-  </si>
-  <si>
-    <t>RL.10197</t>
-  </si>
-  <si>
-    <t>RL.10198</t>
-  </si>
-  <si>
-    <t>RL.10199</t>
-  </si>
-  <si>
     <t>RL.10200</t>
   </si>
   <si>
@@ -11621,6 +11561,78 @@
   </si>
   <si>
     <t>RL.10958</t>
+  </si>
+  <si>
+    <t>RL.10959</t>
+  </si>
+  <si>
+    <t>RL.10960</t>
+  </si>
+  <si>
+    <t>RL.10961</t>
+  </si>
+  <si>
+    <t>RL.10962</t>
+  </si>
+  <si>
+    <t>RL.10963</t>
+  </si>
+  <si>
+    <t>RL.10964</t>
+  </si>
+  <si>
+    <t>RL.10965</t>
+  </si>
+  <si>
+    <t>RL.10966</t>
+  </si>
+  <si>
+    <t>RL.10967</t>
+  </si>
+  <si>
+    <t>RL.10968</t>
+  </si>
+  <si>
+    <t>RL.10969</t>
+  </si>
+  <si>
+    <t>RL.10970</t>
+  </si>
+  <si>
+    <t>RL.10971</t>
+  </si>
+  <si>
+    <t>RL.10972</t>
+  </si>
+  <si>
+    <t>RL.10973</t>
+  </si>
+  <si>
+    <t>RL.10974</t>
+  </si>
+  <si>
+    <t>RL.10975</t>
+  </si>
+  <si>
+    <t>RL.10976</t>
+  </si>
+  <si>
+    <t>RL.10977</t>
+  </si>
+  <si>
+    <t>RL.10978</t>
+  </si>
+  <si>
+    <t>005908386</t>
+  </si>
+  <si>
+    <t>Knights of Malta</t>
+  </si>
+  <si>
+    <t>trent-knightsofmalta</t>
+  </si>
+  <si>
+    <t>RL.10979</t>
   </si>
 </sst>
 </file>
@@ -11656,9 +11668,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11706,8 +11719,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E780" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:E780"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E782" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:E782"/>
   <tableColumns count="5">
     <tableColumn id="1" uniqueName="alephnum" name="alephnum">
       <xmlColumnPr mapId="1" xpath="/data/record/alephnum" xmlDataType="string"/>
@@ -11992,10 +12005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E780"/>
+  <dimension ref="A1:E781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A752" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E780"/>
+    <sheetView tabSelected="1" topLeftCell="A760" workbookViewId="0">
+      <selection activeCell="B781" sqref="B781"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25235,10 +25248,25 @@
         <v>3862</v>
       </c>
     </row>
+    <row r="781" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A781" s="2" t="s">
+        <v>3863</v>
+      </c>
+      <c r="C781" s="1" t="s">
+        <v>3864</v>
+      </c>
+      <c r="D781" s="1" t="s">
+        <v>3865</v>
+      </c>
+      <c r="E781" s="1" t="s">
+        <v>3866</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>